<commit_message>
doc: GR08_MUL test summary
</commit_message>
<xml_diff>
--- a/Tested_asm/Results.xlsx
+++ b/Tested_asm/Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,13 +9,30 @@
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>G08_MUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fault coverage </t>
+  </si>
+  <si>
+    <t>Test coverage</t>
+  </si>
+  <si>
+    <t>Clock cycles</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -32,7 +49,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,23 +57,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -98,7 +145,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +180,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +388,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G11:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.30280000000000001</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.30320000000000003</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
doc: add load_store GR08
</commit_message>
<xml_diff>
--- a/Tested_asm/Results.xlsx
+++ b/Tested_asm/Results.xlsx
@@ -530,7 +530,7 @@
   <dimension ref="D13:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +790,9 @@
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="J31" s="9">
+        <v>0.6018</v>
+      </c>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>

</xml_diff>

<commit_message>
G04 Alu tested --> ok
</commit_message>
<xml_diff>
--- a/Tested_asm/Results.xlsx
+++ b/Tested_asm/Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D2CC19-F4D5-4589-8C80-FB8913493229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3FB7C-F8F4-47B8-A121-2D5141AE86B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -607,28 +607,28 @@
   <dimension ref="D13:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="35.85546875" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.88671875" customWidth="1"/>
+    <col min="7" max="7" width="35.44140625" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="16" width="12.140625" customWidth="1"/>
+    <col min="15" max="16" width="12.109375" customWidth="1"/>
     <col min="22" max="22" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G13" s="1"/>
     </row>
-    <row r="16" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
         <v>0</v>
       </c>
@@ -660,7 +660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G17" s="4" t="s">
         <v>10</v>
       </c>
@@ -678,7 +678,7 @@
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G18" s="4" t="s">
         <v>13</v>
       </c>
@@ -696,7 +696,7 @@
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G19" s="4" t="s">
         <v>14</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G20" s="4" t="s">
         <v>15</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G21" s="4" t="s">
         <v>16</v>
       </c>
@@ -750,7 +750,7 @@
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G22" s="4" t="s">
         <v>17</v>
       </c>
@@ -768,7 +768,7 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G23" s="4" t="s">
         <v>18</v>
       </c>
@@ -786,7 +786,7 @@
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G24" s="4" t="s">
         <v>19</v>
       </c>
@@ -804,7 +804,7 @@
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G25" s="4" t="s">
         <v>20</v>
       </c>
@@ -822,14 +822,16 @@
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H26" s="5">
         <v>32094</v>
       </c>
-      <c r="I26" s="5"/>
+      <c r="I26" s="6">
+        <v>0.3488</v>
+      </c>
       <c r="J26" s="6" t="s">
         <v>34</v>
       </c>
@@ -839,7 +841,7 @@
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G27" s="4" t="s">
         <v>24</v>
       </c>
@@ -857,7 +859,7 @@
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G28" s="4" t="s">
         <v>23</v>
       </c>
@@ -875,7 +877,7 @@
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G29" s="4" t="s">
         <v>22</v>
       </c>
@@ -893,14 +895,16 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G30" s="4" t="s">
         <v>21</v>
       </c>
       <c r="H30" s="5">
         <v>39780</v>
       </c>
-      <c r="I30" s="5"/>
+      <c r="I30" s="6">
+        <v>0.45190000000000002</v>
+      </c>
       <c r="J30" s="6" t="s">
         <v>38</v>
       </c>
@@ -911,7 +915,7 @@
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
     </row>
-    <row r="31" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G31" s="4" t="s">
         <v>11</v>
       </c>
@@ -929,7 +933,7 @@
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
     </row>
-    <row r="32" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G32" s="4" t="s">
         <v>12</v>
       </c>
@@ -947,7 +951,7 @@
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
     </row>
-    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G33" s="9"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
@@ -959,34 +963,34 @@
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
     </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D36" s="7"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
     </row>
-    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G38" s="12"/>
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
       <c r="J38" s="11"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
       <c r="L39" s="7"/>
     </row>
-    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>

</xml_diff>

<commit_message>
G04 test_regs --> ok
</commit_message>
<xml_diff>
--- a/Tested_asm/Results.xlsx
+++ b/Tested_asm/Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3FB7C-F8F4-47B8-A121-2D5141AE86B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D69B462-D017-460F-BD5B-9979610D43A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <dimension ref="D13:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +739,9 @@
       <c r="H21" s="5">
         <v>39590</v>
       </c>
-      <c r="I21" s="5"/>
+      <c r="I21" s="6">
+        <v>0.71499999999999997</v>
+      </c>
       <c r="J21" s="6" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
add G04 results and update the excel
</commit_message>
<xml_diff>
--- a/Tested_asm/Results.xlsx
+++ b/Tested_asm/Results.xlsx
@@ -3,19 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D69B462-D017-460F-BD5B-9979610D43A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9899444-EC01-44D9-8647-4BAD1E59937A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7500" windowHeight="8736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>instance</t>
   </si>
@@ -138,6 +149,21 @@
   </si>
   <si>
     <t>21.54%</t>
+  </si>
+  <si>
+    <t>/if_stage_i</t>
+  </si>
+  <si>
+    <t>/if_stage_i/prefetch_128_prefetch_buffer_i/L0_buffer_i</t>
+  </si>
+  <si>
+    <t>/id_stage_i</t>
+  </si>
+  <si>
+    <t>/id_stage_i/registers_i/riscv_register_file_i</t>
+  </si>
+  <si>
+    <t>/RISCY_PMP_pmp_unit_i</t>
   </si>
 </sst>
 </file>
@@ -604,16 +630,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D13:P40"/>
+  <dimension ref="D13:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="35.88671875" customWidth="1"/>
-    <col min="7" max="7" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.109375" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="14.109375" customWidth="1"/>
@@ -665,9 +691,11 @@
         <v>10</v>
       </c>
       <c r="H17" s="5">
-        <v>171292</v>
-      </c>
-      <c r="I17" s="5"/>
+        <v>269436</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.51870000000000005</v>
+      </c>
       <c r="J17" s="6">
         <v>0.74980000000000002</v>
       </c>
@@ -680,15 +708,15 @@
     </row>
     <row r="18" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G18" s="4" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H18" s="5">
-        <v>10588</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6" t="s">
-        <v>26</v>
-      </c>
+        <v>17028</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.63280000000000003</v>
+      </c>
+      <c r="J18" s="6"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -698,14 +726,16 @@
     </row>
     <row r="19" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" s="5">
-        <v>1628</v>
-      </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5" t="s">
-        <v>27</v>
+        <v>10588</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.71240000000000003</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -716,15 +746,15 @@
     </row>
     <row r="20" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G20" s="4" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="H20" s="5">
-        <v>1504</v>
-      </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="6" t="s">
-        <v>28</v>
-      </c>
+        <v>3780</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.65980000000000005</v>
+      </c>
+      <c r="J20" s="6"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
@@ -734,16 +764,16 @@
     </row>
     <row r="21" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G21" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H21" s="5">
-        <v>39590</v>
+        <v>1628</v>
       </c>
       <c r="I21" s="6">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>29</v>
+        <v>0.47789999999999999</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -754,14 +784,16 @@
     </row>
     <row r="22" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G22" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H22" s="5">
-        <v>4136</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5" t="s">
-        <v>30</v>
+        <v>1504</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.82450000000000001</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -772,15 +804,15 @@
     </row>
     <row r="23" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G23" s="4" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="H23" s="5">
-        <v>2278</v>
-      </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>65582</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.83809999999999996</v>
+      </c>
+      <c r="J23" s="6"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -790,14 +822,16 @@
     </row>
     <row r="24" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G24" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H24" s="5">
-        <v>184</v>
-      </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5" t="s">
-        <v>32</v>
+        <v>39590</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0.96130000000000004</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -808,15 +842,15 @@
     </row>
     <row r="25" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G25" s="4" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="H25" s="5">
-        <v>3222</v>
-      </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>39590</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.96130000000000004</v>
+      </c>
+      <c r="J25" s="6"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
@@ -826,17 +860,18 @@
     </row>
     <row r="26" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G26" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H26" s="5">
-        <v>32094</v>
+        <v>4136</v>
       </c>
       <c r="I26" s="6">
-        <v>0.3488</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>0.75860000000000005</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
@@ -845,14 +880,16 @@
     </row>
     <row r="27" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G27" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H27" s="5">
-        <v>340</v>
-      </c>
-      <c r="I27" s="5"/>
+        <v>2278</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0.38829999999999998</v>
+      </c>
       <c r="J27" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -863,14 +900,16 @@
     </row>
     <row r="28" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G28" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H28" s="5">
-        <v>416</v>
-      </c>
-      <c r="I28" s="5"/>
+        <v>184</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0</v>
+      </c>
       <c r="J28" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -881,14 +920,16 @@
     </row>
     <row r="29" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G29" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H29" s="5">
-        <v>5280</v>
-      </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5" t="s">
-        <v>37</v>
+        <v>3222</v>
+      </c>
+      <c r="I29" s="6">
+        <v>0.35770000000000002</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
@@ -899,18 +940,17 @@
     </row>
     <row r="30" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G30" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H30" s="5">
-        <v>39780</v>
+        <v>32094</v>
       </c>
       <c r="I30" s="6">
-        <v>0.45190000000000002</v>
+        <v>0.88129999999999997</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K30" s="5"/>
+        <v>34</v>
+      </c>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
@@ -919,14 +959,16 @@
     </row>
     <row r="31" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G31" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="H31" s="5">
-        <v>5608</v>
-      </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="6" t="s">
-        <v>39</v>
+        <v>340</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0.94410000000000005</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -937,14 +979,16 @@
     </row>
     <row r="32" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G32" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H32" s="5">
-        <v>30680</v>
-      </c>
-      <c r="I32" s="5"/>
+        <v>416</v>
+      </c>
+      <c r="I32" s="6">
+        <v>0.56969999999999998</v>
+      </c>
       <c r="J32" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -954,49 +998,149 @@
       <c r="P32" s="5"/>
     </row>
     <row r="33" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
+      <c r="G33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="5">
+        <v>5280</v>
+      </c>
+      <c r="I33" s="6">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="5">
+        <v>39780</v>
+      </c>
+      <c r="I34" s="6">
+        <v>0.9395</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="5">
+        <v>5608</v>
+      </c>
+      <c r="I35" s="6">
+        <v>0.67969999999999997</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
     </row>
     <row r="36" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D36" s="7"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
+      <c r="G36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="5">
+        <v>30680</v>
+      </c>
+      <c r="I36" s="6">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
     </row>
     <row r="37" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="11"/>
+      <c r="G37" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" s="5">
+        <v>76610</v>
+      </c>
+      <c r="I37" s="6">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
     </row>
     <row r="38" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="G38" s="12"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="11"/>
-      <c r="L38" s="8"/>
-    </row>
-    <row r="39" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="L39" s="7"/>
-    </row>
-    <row r="40" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+    </row>
+    <row r="41" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D41" s="7"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+    </row>
+    <row r="42" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G43" s="12"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="11"/>
+      <c r="L43" s="8"/>
+    </row>
+    <row r="44" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="L44" s="7"/>
+    </row>
+    <row r="45" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Result and report Updated
</commit_message>
<xml_diff>
--- a/Tested_asm/Results.xlsx
+++ b/Tested_asm/Results.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85EB4BC-08B3-4541-912E-A27F7745D3A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A3A58D-3E6B-4F5D-A3A0-3B480A2999E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
   <si>
     <t>instance</t>
   </si>
@@ -116,7 +117,7 @@
     <t>/ex_stage_i</t>
   </si>
   <si>
-    <t>89.73%</t>
+    <t>NAN</t>
   </si>
 </sst>
 </file>
@@ -663,30 +664,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D13:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P16" activeCellId="1" sqref="G16:H38 P16:P38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.88671875" customWidth="1"/>
     <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
     <col min="22" max="22" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G13" s="1"/>
     </row>
-    <row r="16" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G16" s="2" t="s">
         <v>0</v>
       </c>
@@ -718,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G17" s="20" t="s">
         <v>10</v>
       </c>
@@ -736,11 +737,11 @@
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
       <c r="O17" s="21"/>
-      <c r="P17" s="24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="P17" s="24">
+        <v>0.90180000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G18" s="18" t="s">
         <v>27</v>
       </c>
@@ -759,10 +760,10 @@
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="23">
-        <v>0.68069999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G19" s="19" t="s">
         <v>13</v>
       </c>
@@ -781,10 +782,10 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="23">
-        <v>0.75080000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.76070000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G20" s="19" t="s">
         <v>28</v>
       </c>
@@ -803,10 +804,10 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="23">
-        <v>0.69420000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.70030000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G21" s="19" t="s">
         <v>14</v>
       </c>
@@ -825,10 +826,10 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="23">
-        <v>0.61299999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.64129999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G22" s="19" t="s">
         <v>15</v>
       </c>
@@ -847,10 +848,10 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="23">
-        <v>0.84509999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.85509999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G23" s="18" t="s">
         <v>29</v>
       </c>
@@ -869,10 +870,10 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="23">
-        <v>0.9052</v>
-      </c>
-    </row>
-    <row r="24" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.90649999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G24" s="19" t="s">
         <v>16</v>
       </c>
@@ -891,10 +892,10 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="23">
-        <v>0.98629999999999995</v>
-      </c>
-    </row>
-    <row r="25" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.98760000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G25" s="19" t="s">
         <v>30</v>
       </c>
@@ -913,10 +914,10 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="23">
-        <v>0.98629999999999995</v>
-      </c>
-    </row>
-    <row r="26" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.98760000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G26" s="19" t="s">
         <v>17</v>
       </c>
@@ -935,10 +936,10 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="23">
-        <v>0.80269999999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.8034</v>
+      </c>
+    </row>
+    <row r="27" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G27" s="19" t="s">
         <v>18</v>
       </c>
@@ -957,10 +958,10 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="23">
-        <v>0.40949999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="7:16" x14ac:dyDescent="0.25">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="28" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G28" s="19" t="s">
         <v>19</v>
       </c>
@@ -982,7 +983,7 @@
         <v>7.22E-2</v>
       </c>
     </row>
-    <row r="29" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G29" s="19" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>0.77680000000000005</v>
       </c>
     </row>
-    <row r="30" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G30" s="18" t="s">
         <v>32</v>
       </c>
@@ -1026,7 +1027,7 @@
         <v>0.95909999999999995</v>
       </c>
     </row>
-    <row r="31" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G31" s="19" t="s">
         <v>25</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="32" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G32" s="19" t="s">
         <v>24</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G33" s="19" t="s">
         <v>23</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G34" s="19" t="s">
         <v>22</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>0.95979999999999999</v>
       </c>
     </row>
-    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G35" s="19" t="s">
         <v>21</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>0.97150000000000003</v>
       </c>
     </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G36" s="18" t="s">
         <v>11</v>
       </c>
@@ -1154,10 +1155,10 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="23">
-        <v>0.67769999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
+        <v>0.78120000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G37" s="13" t="s">
         <v>12</v>
       </c>
@@ -1175,9 +1176,11 @@
       <c r="M37" s="14"/>
       <c r="N37" s="14"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-    </row>
-    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="P37" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G38" s="13" t="s">
         <v>31</v>
       </c>
@@ -1195,9 +1198,11 @@
       <c r="M38" s="14"/>
       <c r="N38" s="14"/>
       <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-    </row>
-    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="P38" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G39" s="8"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -1209,34 +1214,34 @@
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
-    <row r="42" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D42" s="6"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G44" s="11"/>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
       <c r="J44" s="10"/>
       <c r="L44" s="7"/>
     </row>
-    <row r="45" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="L45" s="6"/>
     </row>
-    <row r="46" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:16" x14ac:dyDescent="0.3">
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
@@ -1246,4 +1251,277 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC490E4-F839-40D3-B68C-D88DCA976165}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="21">
+        <v>162146</v>
+      </c>
+      <c r="C2" s="24">
+        <v>0.90180000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4">
+        <v>17028</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4">
+        <v>10588</v>
+      </c>
+      <c r="C4" s="23">
+        <v>0.76070000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3780</v>
+      </c>
+      <c r="C5" s="23">
+        <v>0.70030000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1628</v>
+      </c>
+      <c r="C6" s="23">
+        <v>0.64129999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1504</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0.85509999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4">
+        <v>65582</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.90649999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4">
+        <v>39590</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.98760000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4">
+        <v>39590</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0.98760000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4">
+        <v>4136</v>
+      </c>
+      <c r="C11" s="23">
+        <v>0.8034</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2278</v>
+      </c>
+      <c r="C12" s="23">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4">
+        <v>184</v>
+      </c>
+      <c r="C13" s="23">
+        <v>7.22E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3222</v>
+      </c>
+      <c r="C14" s="23">
+        <v>0.77680000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="17">
+        <v>72788</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0.95909999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4">
+        <v>32094</v>
+      </c>
+      <c r="C16" s="23">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="4">
+        <v>340</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4">
+        <v>416</v>
+      </c>
+      <c r="C18" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5280</v>
+      </c>
+      <c r="C19" s="23">
+        <v>0.95979999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="4">
+        <v>39780</v>
+      </c>
+      <c r="C20" s="23">
+        <v>0.97150000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4">
+        <v>5608</v>
+      </c>
+      <c r="C21" s="23">
+        <v>0.78120000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="14">
+        <v>30680</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="14">
+        <v>76610</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>